<commit_message>
Update flora datasets with revised fire traits
</commit_message>
<xml_diff>
--- a/data/Wenk_2023/raw/fire_from_journal_articles_filled.xlsx
+++ b/data/Wenk_2023/raw/fire_from_journal_articles_filled.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208613_ad_unsw_edu_au/Documents/RA Work/AusTraits/scoring_floras/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5208613_ad_unsw_edu_au/Documents/RA Work/AusTraits/austraits.build/data/Wenk_2023/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="8_{C351AC0A-547C-400C-8E06-35D16ED7E5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F21539E7-0DA7-4A84-A86A-F61A12A0A6F2}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="8_{C351AC0A-547C-400C-8E06-35D16ED7E5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D9771A8-994D-42C7-9FC4-6FC2317128A1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2DBD9D12-1BAF-4034-B9E8-C6896CF96D1B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="221">
   <si>
     <t>taxon_name</t>
   </si>
@@ -680,18 +680,9 @@
     <t>biennial short_lived_perennial</t>
   </si>
   <si>
-    <t>obligate_fire_ephemeral</t>
-  </si>
-  <si>
-    <t>life_history_ephemeral</t>
-  </si>
-  <si>
     <t>regenerates after fire; uninterpretable</t>
   </si>
   <si>
-    <t>rootstock</t>
-  </si>
-  <si>
     <t>fleshy_underground_organ</t>
   </si>
   <si>
@@ -702,6 +693,12 @@
   </si>
   <si>
     <t>root_crown</t>
+  </si>
+  <si>
+    <t>basal_buds</t>
+  </si>
+  <si>
+    <t>fire_ephemeral_obligate</t>
   </si>
 </sst>
 </file>
@@ -1056,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EA86EB-DA56-49A2-93DB-A1B998A62099}">
-  <dimension ref="A1:U52"/>
+  <dimension ref="A1:T52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1064,7 @@
     <col min="6" max="6" width="134.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1111,7 @@
         <v>183</v>
       </c>
       <c r="P1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="Q1" t="s">
         <v>198</v>
@@ -1128,11 +1125,8 @@
       <c r="T1" t="s">
         <v>212</v>
       </c>
-      <c r="U1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:20" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1167,7 +1161,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1199,13 +1193,10 @@
         <v>170</v>
       </c>
       <c r="O3" t="s">
-        <v>217</v>
-      </c>
-      <c r="P3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1237,13 +1228,10 @@
         <v>170</v>
       </c>
       <c r="O4" t="s">
-        <v>217</v>
-      </c>
-      <c r="P4" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1278,7 +1266,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1310,13 +1298,10 @@
         <v>170</v>
       </c>
       <c r="O6" t="s">
-        <v>217</v>
-      </c>
-      <c r="P6" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1348,13 +1333,10 @@
         <v>170</v>
       </c>
       <c r="O7" t="s">
-        <v>217</v>
-      </c>
-      <c r="P7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1386,13 +1368,10 @@
         <v>170</v>
       </c>
       <c r="O8" t="s">
-        <v>217</v>
-      </c>
-      <c r="P8" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1424,13 +1403,10 @@
         <v>170</v>
       </c>
       <c r="O9" t="s">
-        <v>217</v>
-      </c>
-      <c r="P9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1462,7 +1438,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1494,7 +1470,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1526,7 +1502,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -1558,7 +1534,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1590,13 +1566,10 @@
         <v>196</v>
       </c>
       <c r="O14" t="s">
-        <v>217</v>
-      </c>
-      <c r="P14" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -1628,13 +1601,10 @@
         <v>196</v>
       </c>
       <c r="O15" t="s">
-        <v>217</v>
-      </c>
-      <c r="P15" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1666,13 +1636,10 @@
         <v>196</v>
       </c>
       <c r="O16" t="s">
-        <v>217</v>
-      </c>
-      <c r="P16" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -1704,7 +1671,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1736,7 +1703,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -1768,7 +1735,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -1800,13 +1767,10 @@
         <v>197</v>
       </c>
       <c r="O20" t="s">
-        <v>217</v>
-      </c>
-      <c r="P20" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -1838,7 +1802,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -1870,7 +1834,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -1902,7 +1866,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -1934,7 +1898,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -1966,7 +1930,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -1998,7 +1962,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -2030,7 +1994,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -2062,7 +2026,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>86</v>
       </c>
@@ -2094,7 +2058,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>88</v>
       </c>
@@ -2126,7 +2090,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -2158,7 +2122,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -2190,7 +2154,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="300" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="300" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>94</v>
       </c>
@@ -2219,7 +2183,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="315" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="315" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>98</v>
       </c>
@@ -2251,7 +2215,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="330" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="330" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>101</v>
       </c>
@@ -2286,7 +2250,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="360" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="360" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>103</v>
       </c>
@@ -2312,10 +2276,10 @@
         <v>107</v>
       </c>
       <c r="I36" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>108</v>
       </c>
@@ -2350,16 +2314,13 @@
         <v>199</v>
       </c>
       <c r="R37" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="S37" t="s">
         <v>202</v>
       </c>
-      <c r="U37" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="315" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:19" ht="315" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>111</v>
       </c>
@@ -2391,7 +2352,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>114</v>
       </c>
@@ -2426,16 +2387,13 @@
         <v>199</v>
       </c>
       <c r="R39" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="S39" t="s">
         <v>202</v>
       </c>
-      <c r="U39" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="255" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:19" ht="255" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -2467,7 +2425,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="345" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="345" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>118</v>
       </c>
@@ -2502,16 +2460,13 @@
         <v>203</v>
       </c>
       <c r="R41" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="S41" t="s">
         <v>202</v>
       </c>
-      <c r="U41" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="409.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>121</v>
       </c>
@@ -2546,7 +2501,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="375" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="375" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>127</v>
       </c>
@@ -2578,13 +2533,13 @@
         <v>170</v>
       </c>
       <c r="O43" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="P43" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>131</v>
       </c>
@@ -2616,7 +2571,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>136</v>
       </c>
@@ -2651,7 +2606,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="300" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="300" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>139</v>
       </c>
@@ -2683,10 +2638,10 @@
         <v>170</v>
       </c>
       <c r="O46" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" ht="300" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="300" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>143</v>
       </c>
@@ -2718,7 +2673,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="330" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="330" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>146</v>
       </c>

</xml_diff>